<commit_message>
Minor changes in Document
</commit_message>
<xml_diff>
--- a/results/result.xlsx
+++ b/results/result.xlsx
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
-  <si>
-    <t>s2-s4</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
   <si>
     <t>2ms</t>
   </si>
   <si>
     <t>26ms</t>
-  </si>
-  <si>
-    <t>s9-13</t>
   </si>
   <si>
     <t>SDN -convergence time</t>
@@ -65,6 +59,18 @@
   </si>
   <si>
     <t>Legacy -convergence time</t>
+  </si>
+  <si>
+    <t>SDN s2-s4</t>
+  </si>
+  <si>
+    <t>SDN s9-13</t>
+  </si>
+  <si>
+    <t>OSPF s2-s4</t>
+  </si>
+  <si>
+    <t>OSPF s9-13</t>
   </si>
 </sst>
 </file>
@@ -203,7 +209,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1021,7 +1027,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sk-SK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="475840576"/>
@@ -1080,7 +1086,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sk-SK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="475839264"/>
@@ -1122,7 +1128,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1159,7 +1165,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="sk-SK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1235,7 +1241,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1254,7 +1260,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s2-s4</c:v>
+                  <c:v>SDN s2-s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1329,7 +1335,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s9-13</c:v>
+                  <c:v>SDN s9-13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1404,7 +1410,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s2-s4</c:v>
+                  <c:v>OSPF s2-s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1479,7 +1485,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s9-13</c:v>
+                  <c:v>OSPF s9-13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1597,7 +1603,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sk-SK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="325501784"/>
@@ -1656,7 +1662,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sk-SK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="325511952"/>
@@ -1698,7 +1704,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1735,7 +1741,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="sk-SK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1816,7 +1822,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1835,7 +1841,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s2-s4</c:v>
+                  <c:v>SDN s2-s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1910,7 +1916,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s9-13</c:v>
+                  <c:v>SDN s9-13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1985,7 +1991,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s2-s4</c:v>
+                  <c:v>OSPF s2-s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2060,7 +2066,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s9-13</c:v>
+                  <c:v>OSPF s9-13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2178,7 +2184,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sk-SK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="325510312"/>
@@ -2237,7 +2243,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sk-SK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="325509328"/>
@@ -2279,7 +2285,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2316,7 +2322,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="sk-SK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2397,7 +2403,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2416,7 +2422,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s2-s4</c:v>
+                  <c:v>SDN s2-s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2491,7 +2497,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s9-13</c:v>
+                  <c:v>SDN s9-13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2566,7 +2572,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s2-s4</c:v>
+                  <c:v>OSPF s2-s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2641,7 +2647,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s9-13</c:v>
+                  <c:v>OSPF s9-13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2759,7 +2765,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sk-SK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="507752416"/>
@@ -2818,7 +2824,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sk-SK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="507752088"/>
@@ -2860,7 +2866,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2897,7 +2903,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="sk-SK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2973,7 +2979,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2992,7 +2998,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s2-s4</c:v>
+                  <c:v>SDN s2-s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3067,7 +3073,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s9-13</c:v>
+                  <c:v>SDN s9-13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3142,7 +3148,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s2-s4</c:v>
+                  <c:v>OSPF s2-s4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3217,7 +3223,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s9-13</c:v>
+                  <c:v>OSPF s9-13</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3335,7 +3341,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sk-SK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="459273864"/>
@@ -3394,7 +3400,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sk-SK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="459272880"/>
@@ -3436,7 +3442,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3473,7 +3479,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="sk-SK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6719,7 +6725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BFFB51-E441-4EFF-880D-76F05951A208}">
   <dimension ref="B1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
@@ -6737,30 +6743,30 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -7630,7 +7636,7 @@
   <dimension ref="C3:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7654,7 +7660,7 @@
   <sheetData>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -7665,7 +7671,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -7678,25 +7684,25 @@
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -7704,102 +7710,102 @@
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
       <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
       <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
-        <v>2</v>
-      </c>
       <c r="I5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
         <v>1</v>
       </c>
-      <c r="J5" t="s">
-        <v>2</v>
-      </c>
       <c r="K5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>1</v>
       </c>
-      <c r="L5" t="s">
-        <v>2</v>
-      </c>
       <c r="M5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
         <v>1</v>
       </c>
-      <c r="N5" t="s">
-        <v>2</v>
-      </c>
       <c r="O5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
         <v>1</v>
       </c>
-      <c r="P5" t="s">
-        <v>2</v>
-      </c>
       <c r="Q5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
         <v>1</v>
-      </c>
-      <c r="R5" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="K6" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="N6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="O6" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P6" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="R6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">

</xml_diff>